<commit_message>
Got dates and locations for 17-18 and 0.1-0.3
</commit_message>
<xml_diff>
--- a/Table-X-SurfaceVariables.xlsx
+++ b/Table-X-SurfaceVariables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Year</t>
   </si>
@@ -69,7 +69,67 @@
     <t>Distance (km)</t>
   </si>
   <si>
-    <t>Stations</t>
+    <t>0.15-0.25 Stations</t>
+  </si>
+  <si>
+    <t>17-18° Stations</t>
+  </si>
+  <si>
+    <t>35-41</t>
+  </si>
+  <si>
+    <t>26-30</t>
+  </si>
+  <si>
+    <t>0.15-0.25 Latitude</t>
+  </si>
+  <si>
+    <t>17-18° Latitude</t>
+  </si>
+  <si>
+    <t>34.25-35.75</t>
+  </si>
+  <si>
+    <t>32.25-33</t>
+  </si>
+  <si>
+    <t>0.15-0.25 Times</t>
+  </si>
+  <si>
+    <t>17-18° Times</t>
+  </si>
+  <si>
+    <t>3/29-4/3</t>
+  </si>
+  <si>
+    <t>3/28-3/29</t>
+  </si>
+  <si>
+    <t>3/19-3/20</t>
+  </si>
+  <si>
+    <t>27-30</t>
+  </si>
+  <si>
+    <t>18-22</t>
+  </si>
+  <si>
+    <t>31.25-32.25</t>
+  </si>
+  <si>
+    <t>21-25</t>
+  </si>
+  <si>
+    <t>33-35</t>
+  </si>
+  <si>
+    <t>35-35.75</t>
+  </si>
+  <si>
+    <t>3/22-3/24</t>
+  </si>
+  <si>
+    <t>32.5-33.5</t>
   </si>
 </sst>
 </file>
@@ -163,18 +223,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,12 +253,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -517,72 +606,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="12" max="12" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16.1640625" customWidth="1"/>
+    <col min="15" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:17" ht="16">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:17">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.15</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.25</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>18</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>17.5</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>17</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="2">
+    <row r="3" spans="1:17">
+      <c r="A3" s="1">
         <v>2008</v>
       </c>
       <c r="B3">
@@ -603,9 +713,27 @@
       <c r="G3">
         <v>32.799999999999997</v>
       </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="2">
+    <row r="4" spans="1:17">
+      <c r="A4" s="1">
         <v>2009</v>
       </c>
       <c r="B4">
@@ -626,9 +754,27 @@
       <c r="G4">
         <v>33.04</v>
       </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>41719</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="2">
+    <row r="5" spans="1:17">
+      <c r="A5" s="1">
         <v>2011</v>
       </c>
       <c r="B5">
@@ -648,6 +794,24 @@
       </c>
       <c r="G5">
         <v>32.79</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>41718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added prototype code and figures for Time series of 30-36 lat box, positions of SST and TZCF, and TempFluor profies at SST front
</commit_message>
<xml_diff>
--- a/Table-X-SurfaceVariables.xlsx
+++ b/Table-X-SurfaceVariables.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Frontal Locations" sheetId="1" r:id="rId1"/>
+    <sheet name="Distance" sheetId="2" r:id="rId2"/>
+    <sheet name="Stations and Times" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Year</t>
   </si>
@@ -130,6 +132,51 @@
   </si>
   <si>
     <t>32.5-33.5</t>
+  </si>
+  <si>
+    <t>36*</t>
+  </si>
+  <si>
+    <t>35.75*</t>
+  </si>
+  <si>
+    <t>36.5*</t>
+  </si>
+  <si>
+    <t>*Intense Clouds</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>3/23-3/30</t>
+  </si>
+  <si>
+    <t>3/26-4/1</t>
+  </si>
+  <si>
+    <t>3/19-3/25</t>
+  </si>
+  <si>
+    <t>3/16-3/22</t>
+  </si>
+  <si>
+    <t>3/14-3/20</t>
+  </si>
+  <si>
+    <t>3/11-3/17</t>
+  </si>
+  <si>
+    <t>SST</t>
+  </si>
+  <si>
+    <t>3/20-3/29</t>
+  </si>
+  <si>
+    <t>Chla</t>
+  </si>
+  <si>
+    <t>3/19-4/3</t>
   </si>
 </sst>
 </file>
@@ -223,7 +270,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -243,8 +290,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -257,8 +320,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -268,6 +335,14 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -277,6 +352,14 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,219 +689,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="12" max="12" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="16.1640625" customWidth="1"/>
-    <col min="15" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:9" ht="16">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3">
         <v>0.15</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>0.2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>0.25</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>18</v>
       </c>
-      <c r="F2" s="3">
+      <c r="H2" s="3">
         <v>17.5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="I2" s="3">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>2008</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="7"/>
+      <c r="C3">
         <v>32.340000000000003</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>32.83</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>33.24</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>32.29</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>32.76</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>32.799999999999997</v>
       </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2009</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7"/>
+      <c r="C4">
         <v>34.79</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>36.22</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>36.5</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>31.73</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>31.78</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>33.04</v>
       </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>41719</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>2011</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="7"/>
+      <c r="C5">
         <v>32.9</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>34.020000000000003</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>34.24</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>31.58</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>32.69</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>32.79</v>
       </c>
-      <c r="L5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>41718</v>
+    </row>
+    <row r="8" spans="1:9" ht="16">
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="3">
+        <v>18</v>
+      </c>
+      <c r="H9" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="D10">
+        <v>35.64</v>
+      </c>
+      <c r="E10">
+        <v>36.85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10">
+        <v>33.24</v>
+      </c>
+      <c r="H10">
+        <v>33.32</v>
+      </c>
+      <c r="I10">
+        <v>33.42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <v>30.86</v>
+      </c>
+      <c r="H11">
+        <v>31.54</v>
+      </c>
+      <c r="I11">
+        <v>32.049999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>34.08</v>
+      </c>
+      <c r="D12">
+        <v>34.340000000000003</v>
+      </c>
+      <c r="E12">
+        <v>35.340000000000003</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12">
+        <v>31.81</v>
+      </c>
+      <c r="H12">
+        <v>32.159999999999997</v>
+      </c>
+      <c r="I12">
+        <v>32.69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:K1"/>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="G8:I8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -828,4 +947,202 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5">
+        <v>41719</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="5">
+        <v>41718</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work on figure 4 and adjustment to Station table and Working.mat
</commit_message>
<xml_diff>
--- a/Table-X-SurfaceVariables.xlsx
+++ b/Table-X-SurfaceVariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="12100" yWindow="80" windowWidth="39120" windowHeight="26880" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontal Locations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Year</t>
   </si>
@@ -89,51 +89,12 @@
     <t>17-18° Latitude</t>
   </si>
   <si>
-    <t>34.25-35.75</t>
-  </si>
-  <si>
-    <t>32.25-33</t>
-  </si>
-  <si>
     <t>0.15-0.25 Times</t>
   </si>
   <si>
     <t>17-18° Times</t>
   </si>
   <si>
-    <t>3/29-4/3</t>
-  </si>
-  <si>
-    <t>3/28-3/29</t>
-  </si>
-  <si>
-    <t>3/19-3/20</t>
-  </si>
-  <si>
-    <t>27-30</t>
-  </si>
-  <si>
-    <t>18-22</t>
-  </si>
-  <si>
-    <t>31.25-32.25</t>
-  </si>
-  <si>
-    <t>21-25</t>
-  </si>
-  <si>
-    <t>33-35</t>
-  </si>
-  <si>
-    <t>35-35.75</t>
-  </si>
-  <si>
-    <t>3/22-3/24</t>
-  </si>
-  <si>
-    <t>32.5-33.5</t>
-  </si>
-  <si>
     <t>36*</t>
   </si>
   <si>
@@ -177,12 +138,60 @@
   </si>
   <si>
     <t>3/19-4/3</t>
+  </si>
+  <si>
+    <t>32.00°-32.75°N</t>
+  </si>
+  <si>
+    <t>26-29</t>
+  </si>
+  <si>
+    <t>16-22</t>
+  </si>
+  <si>
+    <t>30.75°-32.25°N</t>
+  </si>
+  <si>
+    <t>20-25</t>
+  </si>
+  <si>
+    <t>31.00°-32.25°N</t>
+  </si>
+  <si>
+    <t>March 20-21, 2011</t>
+  </si>
+  <si>
+    <t>March 28-29, 2008</t>
+  </si>
+  <si>
+    <t>March 29 - April 3, 2008</t>
+  </si>
+  <si>
+    <t>33-36</t>
+  </si>
+  <si>
+    <t>35.00°-36.00°N</t>
+  </si>
+  <si>
+    <t>March 22 - 24, 2009</t>
+  </si>
+  <si>
+    <t>March 19 - 20, 2011</t>
+  </si>
+  <si>
+    <t>32.50°-33.50°N</t>
+  </si>
+  <si>
+    <t>34.25°-35.75°N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -270,7 +279,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -306,8 +315,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,13 +330,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -343,6 +362,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -360,6 +380,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -739,7 +760,7 @@
       <c r="A3" s="1">
         <v>2008</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>32.340000000000003</v>
       </c>
@@ -763,7 +784,7 @@
       <c r="A4" s="1">
         <v>2009</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>34.79</v>
       </c>
@@ -787,7 +808,7 @@
       <c r="A5" s="1">
         <v>2011</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>32.9</v>
       </c>
@@ -825,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>0.15</v>
@@ -837,7 +858,7 @@
         <v>0.25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G9" s="3">
         <v>18</v>
@@ -851,7 +872,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="B10" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>34.450000000000003</v>
@@ -863,7 +884,7 @@
         <v>36.85</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G10">
         <v>33.24</v>
@@ -877,19 +898,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="B11" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <v>30.86</v>
@@ -903,7 +924,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="B12" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>34.08</v>
@@ -915,7 +936,7 @@
         <v>35.340000000000003</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="G12">
         <v>31.81</v>
@@ -929,7 +950,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="C16" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1014,131 +1035,133 @@
   <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
       <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="C4" s="8">
+        <v>39893</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="5">
-        <v>41719</v>
+        <v>41</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5">
-        <v>41718</v>
+        <v>44</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added temp and fluor mean profiles for STFZ. Changed station list
</commit_message>
<xml_diff>
--- a/Table-X-SurfaceVariables.xlsx
+++ b/Table-X-SurfaceVariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12100" yWindow="80" windowWidth="39120" windowHeight="26880" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontal Locations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Year</t>
   </si>
@@ -184,13 +184,34 @@
   <si>
     <t>34.25°-35.75°N</t>
   </si>
+  <si>
+    <t>By EYE</t>
+  </si>
+  <si>
+    <t>By PROFILE</t>
+  </si>
+  <si>
+    <t>27-29</t>
+  </si>
+  <si>
+    <t>32.25°-32.75°N</t>
+  </si>
+  <si>
+    <t>18-22</t>
+  </si>
+  <si>
+    <t>31.25°-32.25°N</t>
+  </si>
+  <si>
+    <t>21-25</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -279,8 +300,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -331,20 +354,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +386,7 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -381,6 +405,7 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -719,17 +744,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -829,17 +854,17 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="16">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
@@ -981,12 +1006,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
@@ -1032,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1047,6 +1072,11 @@
     <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>9</v>
@@ -1074,7 +1104,7 @@
       <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="s">
@@ -1083,7 +1113,7 @@
       <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H3" t="s">
@@ -1100,7 +1130,7 @@
       <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>39893</v>
       </c>
       <c r="D4" t="s">
@@ -1109,7 +1139,7 @@
       <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H4" t="s">
@@ -1126,7 +1156,7 @@
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D5" t="s">
@@ -1135,8 +1165,13 @@
       <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1157,6 +1192,66 @@
       </c>
       <c r="F9" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7">
+        <v>39893</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>